<commit_message>
add command splitxlsx #32
</commit_message>
<xml_diff>
--- a/testdata/accounts.xlsx
+++ b/testdata/accounts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="names" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -36,7 +36,10 @@
     <t xml:space="preserve">username</t>
   </si>
   <si>
-    <t xml:space="preserve">Rob Pike</t>
+    <t xml:space="preserve">Rob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pike</t>
   </si>
   <si>
     <t xml:space="preserve">rob</t>
@@ -100,7 +103,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -121,6 +124,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -165,9 +175,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -193,105 +215,104 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.54"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="0" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>12</v>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="0" t="s">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3" t="n">
         <v>123</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:C2"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -309,52 +330,52 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="3" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>15</v>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="0" t="n">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="n">
         <v>11111</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="0" t="n">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="n">
         <v>12345</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="0" t="n">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="n">
         <v>22222</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="0" t="n">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="n">
         <v>999999</v>
       </c>
     </row>
@@ -376,53 +397,54 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="3" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>22</v>
+      <c r="B5" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>